<commit_message>
working fine till now
</commit_message>
<xml_diff>
--- a/Python_with_excel/excel_files/Exported.xlsx
+++ b/Python_with_excel/excel_files/Exported.xlsx
@@ -1631,7 +1631,7 @@
         </is>
       </c>
       <c r="M7" s="52" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N7" s="99" t="inlineStr">
         <is>
@@ -2490,7 +2490,7 @@
         </is>
       </c>
       <c r="M19" s="52" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="N19" s="99" t="inlineStr">
         <is>
@@ -2776,7 +2776,7 @@
         </is>
       </c>
       <c r="M23" s="52" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N23" s="99" t="inlineStr">
         <is>
@@ -3062,7 +3062,7 @@
         </is>
       </c>
       <c r="M27" s="52" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="N27" s="99" t="inlineStr">
         <is>
@@ -3486,7 +3486,7 @@
         </is>
       </c>
       <c r="M33" s="52" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="N33" s="99" t="inlineStr">
         <is>
@@ -5320,7 +5320,7 @@
         </is>
       </c>
       <c r="M54" s="52" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N54" s="99" t="inlineStr">
         <is>
@@ -5692,7 +5692,7 @@
         </is>
       </c>
       <c r="M58" s="52" t="n">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="N58" s="99" t="inlineStr">
         <is>
@@ -6138,7 +6138,7 @@
         </is>
       </c>
       <c r="M63" s="52" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="N63" s="99" t="inlineStr">
         <is>
@@ -6314,7 +6314,7 @@
         </is>
       </c>
       <c r="M65" s="52" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N65" s="99" t="inlineStr">
         <is>
@@ -6666,7 +6666,7 @@
         </is>
       </c>
       <c r="M69" s="52" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N69" s="99" t="inlineStr">
         <is>
@@ -6842,7 +6842,7 @@
         </is>
       </c>
       <c r="M71" s="52" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N71" s="99" t="inlineStr">
         <is>
@@ -7456,7 +7456,7 @@
         </is>
       </c>
       <c r="M78" s="52" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="N78" s="99" t="inlineStr">
         <is>
@@ -7544,7 +7544,7 @@
         </is>
       </c>
       <c r="M79" s="52" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N79" s="99" t="inlineStr">
         <is>
@@ -7632,7 +7632,7 @@
         </is>
       </c>
       <c r="M80" s="52" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="N80" s="99" t="inlineStr">
         <is>
@@ -12497,7 +12497,7 @@
         </is>
       </c>
       <c r="M136" s="52" t="n">
-        <v>315</v>
+        <v>235</v>
       </c>
       <c r="N136" s="99" t="inlineStr">
         <is>

</xml_diff>